<commit_message>
Hover function is done
Hover of menu and social media has been done
</commit_message>
<xml_diff>
--- a/Behat Automated Testing/Automation task/MP_PROD_automated_sanity_check_scenario.xlsx
+++ b/Behat Automated Testing/Automation task/MP_PROD_automated_sanity_check_scenario.xlsx
@@ -1361,7 +1361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="103">
   <si>
     <t>Submit CV</t>
   </si>
@@ -1651,9 +1651,6 @@
     <t>Hover MegaMenu</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>WIP</t>
   </si>
   <si>
@@ -1667,6 +1664,12 @@
   </si>
   <si>
     <t>Would work after hover</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Hover is Done</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1712,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1764,6 +1767,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1801,7 +1810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1836,9 +1845,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1852,6 +1858,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2148,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:G22"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2179,10 +2190,10 @@
         <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -2221,7 +2232,7 @@
         <v>74</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>92</v>
@@ -2237,7 +2248,7 @@
         <v>86</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>92</v>
@@ -2275,7 +2286,7 @@
         <v>86</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>92</v>
@@ -2302,7 +2313,7 @@
         <v>86</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>92</v>
@@ -2353,10 +2364,10 @@
         <v>74</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2391,8 +2402,8 @@
         <v>74</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="3"/>
@@ -2404,8 +2415,8 @@
         <v>74</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="3"/>
@@ -2417,8 +2428,8 @@
         <v>74</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3"/>
@@ -2430,8 +2441,8 @@
         <v>74</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3"/>
@@ -2443,8 +2454,8 @@
         <v>74</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3"/>
@@ -2456,8 +2467,8 @@
         <v>74</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3"/>
@@ -2469,8 +2480,8 @@
         <v>74</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3"/>
@@ -2482,8 +2493,8 @@
         <v>74</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3"/>
@@ -2495,8 +2506,8 @@
         <v>74</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
@@ -2565,11 +2576,11 @@
       <c r="E27" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G27" s="25" t="s">
-        <v>101</v>
+      <c r="G27" s="24" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2584,8 +2595,8 @@
       <c r="E28" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="25"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3"/>
@@ -2599,8 +2610,8 @@
       <c r="E29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="25"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3"/>
@@ -2614,8 +2625,8 @@
       <c r="E30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="25"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3"/>
@@ -2629,8 +2640,8 @@
       <c r="E31" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="25"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3"/>
@@ -2644,8 +2655,8 @@
       <c r="E32" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="25"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
@@ -2766,11 +2777,11 @@
       <c r="E42" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" s="20" t="s">
         <v>94</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2785,7 +2796,7 @@
       <c r="E43" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="21"/>
+      <c r="F43" s="20"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="3"/>
@@ -2815,7 +2826,7 @@
       <c r="E45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F45" s="21"/>
+      <c r="F45" s="20"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="3"/>
@@ -2829,7 +2840,7 @@
       <c r="E46" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F46" s="21"/>
+      <c r="F46" s="20"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="3"/>
@@ -2843,7 +2854,7 @@
       <c r="E47" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F47" s="21"/>
+      <c r="F47" s="20"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="3"/>
@@ -2857,7 +2868,7 @@
       <c r="E48" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F48" s="21"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="3" t="s">
@@ -2949,8 +2960,8 @@
       <c r="E55" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F55" s="22" t="s">
-        <v>98</v>
+      <c r="F55" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2965,7 +2976,7 @@
       <c r="E56" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F56" s="22"/>
+      <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="3"/>
@@ -2979,7 +2990,7 @@
       <c r="E57" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F57" s="22"/>
+      <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="3"/>
@@ -2993,7 +3004,7 @@
       <c r="E58" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F58" s="22"/>
+      <c r="F58" s="21"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3"/>
@@ -3007,7 +3018,7 @@
       <c r="E59" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F59" s="22"/>
+      <c r="F59" s="21"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="3"/>
@@ -3021,7 +3032,7 @@
       <c r="E60" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="22"/>
+      <c r="F60" s="21"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="3"/>
@@ -3035,7 +3046,7 @@
       <c r="E61" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F61" s="22"/>
+      <c r="F61" s="21"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="3"/>
@@ -3049,7 +3060,7 @@
       <c r="E62" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="22"/>
+      <c r="F62" s="21"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="3"/>
@@ -3063,7 +3074,7 @@
       <c r="E63" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F63" s="22"/>
+      <c r="F63" s="21"/>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="3"/>
@@ -3077,7 +3088,7 @@
       <c r="E64" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F64" s="22"/>
+      <c r="F64" s="21"/>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="3" t="s">
@@ -3095,9 +3106,9 @@
       <c r="E65" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F65" s="21"/>
+      <c r="F65" s="20"/>
       <c r="G65" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3110,7 +3121,7 @@
         <v>74</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>93</v>
@@ -3132,9 +3143,9 @@
       <c r="E67" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F67" s="21"/>
+      <c r="F67" s="20"/>
       <c r="G67" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3147,7 +3158,7 @@
         <v>74</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>93</v>
@@ -3187,18 +3198,21 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="3"/>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="C72" s="26"/>
+      <c r="D72" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F72" s="27" t="s">
         <v>94</v>
+      </c>
+      <c r="G72" s="27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:7">

</xml_diff>

<commit_message>
Job apply LinkedIn completed
</commit_message>
<xml_diff>
--- a/Behat Automated Testing/Automation task/MP_PROD_automated_sanity_check_scenario.xlsx
+++ b/Behat Automated Testing/Automation task/MP_PROD_automated_sanity_check_scenario.xlsx
@@ -143,189 +143,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NEGATIVE TESTS:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>First Name:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank, Numeric, Special Characters.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Last Name:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank, Numeric, Special Characters.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Email:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank, Invalid
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Job title:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Location :</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Blank
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sector:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Job Type:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attach CV:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Over 400kb, Invalid format.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C13" authorId="0">
       <text>
         <r>
@@ -336,37 +153,56 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>NEGATIVE TESTS:
-Name:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank, Enter numbers/special characters.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Last name:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank, Enter numbers/special characters.
+          <t>NEGATIVE TESTS:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>First Name:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank, Numeric, Special Characters.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Last Name:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank, Numeric, Special Characters.
 </t>
         </r>
         <r>
@@ -386,47 +222,107 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Blank, Existing user email, incorrectly fomatted email.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Password: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Blank, Less than 6 characters.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verify Pasword:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Blank, missmatch to the original password.</t>
+          <t xml:space="preserve"> Blank, Invalid
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Job title:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Location :</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Blank
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sector:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Job Type:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attach CV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Over 400kb, Invalid format.</t>
         </r>
       </text>
     </comment>
@@ -440,17 +336,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">NEGATIVE TESTS:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t>NEGATIVE TESTS:
+Name:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank, Enter numbers/special characters.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Last name:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank, Enter numbers/special characters.
 </t>
         </r>
         <r>
@@ -470,27 +386,47 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Blank, Unrecognised
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Password</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>: Blank.</t>
+          <t xml:space="preserve"> Blank, Existing user email, incorrectly fomatted email.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Password: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Blank, Less than 6 characters.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Verify Pasword:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank, missmatch to the original password.</t>
         </r>
       </text>
     </comment>
@@ -499,6 +435,70 @@
         <r>
           <rPr>
             <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NEGATIVE TESTS:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Email:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Blank, Unrecognised
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Password</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: Blank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -668,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
+    <comment ref="C21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -715,7 +715,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C24" authorId="0">
+    <comment ref="C25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -758,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0">
+    <comment ref="C28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -821,7 +821,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0">
+    <comment ref="C33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -884,7 +884,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="0">
+    <comment ref="C38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -988,7 +988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C65" authorId="0">
+    <comment ref="C66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1173,7 +1173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C67" authorId="0">
+    <comment ref="C68" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1361,7 +1361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="105">
   <si>
     <t>Submit CV</t>
   </si>
@@ -1670,6 +1670,12 @@
   </si>
   <si>
     <t>Hover is Done</t>
+  </si>
+  <si>
+    <t>Job apply with Linnked in For External Job apply</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1718,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1767,12 +1773,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1810,7 +1810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1846,11 +1846,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1863,6 +1858,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2157,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD95"/>
+  <dimension ref="A1:AD96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2305,43 +2304,47 @@
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="16" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:30">
-      <c r="A11" s="3" t="s">
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:30">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="18" t="s">
-        <v>64</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>74</v>
@@ -2351,184 +2354,186 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:30">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="25" t="s">
+      <c r="D14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-    </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="3"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="14" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="C16" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="C17" s="14" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
       <c r="C18" s="14" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3"/>
       <c r="B19" s="6"/>
       <c r="C19" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="3" t="s">
+      <c r="D23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="18" t="s">
-        <v>53</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>74</v>
@@ -2539,55 +2544,47 @@
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="3" t="s">
+      <c r="D26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>100</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="C28" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>86</v>
@@ -2595,14 +2592,18 @@
       <c r="E28" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="27"/>
+      <c r="F28" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>86</v>
@@ -2610,14 +2611,14 @@
       <c r="E29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="27"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>86</v>
@@ -2625,14 +2626,14 @@
       <c r="E30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="27"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>86</v>
@@ -2640,14 +2641,14 @@
       <c r="E31" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="27"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>86</v>
@@ -2655,29 +2656,33 @@
       <c r="E32" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="27"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C34" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="3"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="16" t="s">
-        <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>74</v>
@@ -2688,7 +2693,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
       <c r="C35" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>74</v>
@@ -2697,9 +2702,9 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>74</v>
@@ -2710,7 +2715,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>74</v>
@@ -2721,7 +2726,7 @@
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>74</v>
@@ -2732,7 +2737,7 @@
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>74</v>
@@ -2743,7 +2748,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>74</v>
@@ -2754,41 +2759,33 @@
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="3" t="s">
+      <c r="D42" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="3"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>86</v>
@@ -2797,14 +2794,17 @@
         <v>88</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="13" t="s">
-        <v>43</v>
+      <c r="C44" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>86</v>
@@ -2812,7 +2812,7 @@
       <c r="E44" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="20" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
       <c r="A45" s="3"/>
       <c r="B45" s="6"/>
       <c r="C45" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>86</v>
@@ -2828,13 +2828,15 @@
       <c r="E45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F45" s="20"/>
+      <c r="F45" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="3"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="12" t="s">
-        <v>45</v>
+      <c r="C46" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>86</v>
@@ -2848,7 +2850,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="6"/>
       <c r="C47" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>86</v>
@@ -2856,15 +2858,13 @@
       <c r="E47" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F47" s="20" t="s">
-        <v>93</v>
-      </c>
+      <c r="F47" s="20"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="3"/>
       <c r="B48" s="6"/>
       <c r="C48" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>86</v>
@@ -2877,20 +2877,19 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>86</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2898,45 +2897,53 @@
         <v>84</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C51" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="16" t="s">
-        <v>56</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="3"/>
-      <c r="B52" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="B52" s="4"/>
       <c r="C52" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="3"/>
-      <c r="B53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C53" s="16" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -2945,36 +2952,29 @@
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="3"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C56" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="3"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="14" t="s">
-        <v>30</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>86</v>
@@ -2982,13 +2982,15 @@
       <c r="E56" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F56" s="24"/>
+      <c r="F56" s="21" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="3"/>
-      <c r="B57" s="6"/>
+      <c r="B57" s="4"/>
       <c r="C57" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>86</v>
@@ -2996,13 +2998,13 @@
       <c r="E57" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F57" s="24"/>
+      <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
+      <c r="B58" s="6"/>
       <c r="C58" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>86</v>
@@ -3010,13 +3012,13 @@
       <c r="E58" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F58" s="24"/>
+      <c r="F58" s="21"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>86</v>
@@ -3024,13 +3026,13 @@
       <c r="E59" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F59" s="24"/>
+      <c r="F59" s="21"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D60" s="14" t="s">
         <v>86</v>
@@ -3038,13 +3040,13 @@
       <c r="E60" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="24"/>
+      <c r="F60" s="21"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D61" s="14" t="s">
         <v>86</v>
@@ -3052,13 +3054,13 @@
       <c r="E61" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F61" s="24"/>
+      <c r="F61" s="21"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="3"/>
-      <c r="B62" s="6"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D62" s="14" t="s">
         <v>86</v>
@@ -3066,13 +3068,13 @@
       <c r="E62" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="24"/>
+      <c r="F62" s="21"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
       <c r="C63" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>86</v>
@@ -3080,13 +3082,13 @@
       <c r="E63" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F63" s="24"/>
+      <c r="F63" s="21"/>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="3"/>
       <c r="B64" s="6"/>
       <c r="C64" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>86</v>
@@ -3094,148 +3096,159 @@
       <c r="E64" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F64" s="24"/>
+      <c r="F64" s="21"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="3"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="21"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C66" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D66" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F65" s="20"/>
-      <c r="G65" s="2" t="s">
+      <c r="F66" s="20"/>
+      <c r="G66" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="16" t="s">
+    <row r="67" spans="1:7">
+      <c r="A67" s="3"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E66" s="5" t="s">
+      <c r="D67" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="3" t="s">
+    <row r="68" spans="1:7">
+      <c r="A68" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B68" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C68" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D68" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="2" t="s">
+      <c r="F68" s="20"/>
+      <c r="G68" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="3"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="16" t="s">
+    <row r="69" spans="1:7">
+      <c r="A69" s="3"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E68" s="5" t="s">
+      <c r="D69" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:7">
+      <c r="A70" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C70" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="3"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="16" t="s">
+      <c r="D70" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="3"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="B71" s="11"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
+      <c r="D71" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="3"/>
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="11"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="3"/>
+      <c r="B73" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E72" s="22" t="s">
+      <c r="C73" s="16"/>
+      <c r="D73" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F72" s="23" t="s">
+      <c r="F73" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G72" s="23" t="s">
+      <c r="G73" s="26" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="B73" s="11"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:7">
       <c r="B74" s="11"/>
       <c r="C74" s="7"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
     </row>
     <row r="75" spans="1:7">
+      <c r="B75" s="11"/>
       <c r="C75" s="7"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="B76" s="11"/>
+      <c r="C76" s="7"/>
     </row>
     <row r="77" spans="1:7">
       <c r="B77" s="11"/>
@@ -3261,8 +3274,8 @@
     <row r="84" spans="2:2">
       <c r="B84" s="11"/>
     </row>
-    <row r="86" spans="2:2">
-      <c r="B86" s="11"/>
+    <row r="85" spans="2:2">
+      <c r="B85" s="11"/>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="11"/>
@@ -3291,13 +3304,16 @@
     <row r="95" spans="2:2">
       <c r="B95" s="11"/>
     </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F55:F64"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="F13:F22"/>
-    <mergeCell ref="G13:G22"/>
-    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F56:F65"/>
+    <mergeCell ref="F28:F33"/>
+    <mergeCell ref="F14:F23"/>
+    <mergeCell ref="G14:G23"/>
+    <mergeCell ref="G28:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
My Page Task Allocation change
</commit_message>
<xml_diff>
--- a/Behat Automated Testing/Automation task/MP_PROD_automated_sanity_check_scenario.xlsx
+++ b/Behat Automated Testing/Automation task/MP_PROD_automated_sanity_check_scenario.xlsx
@@ -1846,6 +1846,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1858,10 +1862,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2158,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2380,10 +2380,10 @@
         <v>74</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="23"/>
+      <c r="F14" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="25"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -2418,8 +2418,8 @@
         <v>74</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="3"/>
@@ -2431,8 +2431,8 @@
         <v>74</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3"/>
@@ -2444,8 +2444,8 @@
         <v>74</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3"/>
@@ -2457,8 +2457,8 @@
         <v>74</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3"/>
@@ -2470,8 +2470,8 @@
         <v>74</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3"/>
@@ -2483,8 +2483,8 @@
         <v>74</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3"/>
@@ -2496,8 +2496,8 @@
         <v>74</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3"/>
@@ -2509,8 +2509,8 @@
         <v>74</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3"/>
@@ -2522,8 +2522,8 @@
         <v>74</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
@@ -2592,10 +2592,10 @@
       <c r="E28" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="26" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2611,8 +2611,8 @@
       <c r="E29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3"/>
@@ -2626,8 +2626,8 @@
       <c r="E30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3"/>
@@ -2641,8 +2641,8 @@
       <c r="E31" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3"/>
@@ -2656,8 +2656,8 @@
       <c r="E32" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="3"/>
@@ -2671,8 +2671,8 @@
       <c r="E33" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
@@ -2982,7 +2982,7 @@
       <c r="E56" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F56" s="23" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2998,7 +2998,7 @@
       <c r="E57" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F57" s="21"/>
+      <c r="F57" s="23"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="3"/>
@@ -3012,7 +3012,7 @@
       <c r="E58" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F58" s="21"/>
+      <c r="F58" s="23"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3"/>
@@ -3026,7 +3026,7 @@
       <c r="E59" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F59" s="21"/>
+      <c r="F59" s="23"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="3"/>
@@ -3040,7 +3040,7 @@
       <c r="E60" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="21"/>
+      <c r="F60" s="23"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="3"/>
@@ -3054,7 +3054,7 @@
       <c r="E61" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F61" s="21"/>
+      <c r="F61" s="23"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="3"/>
@@ -3068,7 +3068,7 @@
       <c r="E62" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="21"/>
+      <c r="F62" s="23"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="3"/>
@@ -3082,7 +3082,7 @@
       <c r="E63" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F63" s="21"/>
+      <c r="F63" s="23"/>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="3"/>
@@ -3096,7 +3096,7 @@
       <c r="E64" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F64" s="21"/>
+      <c r="F64" s="23"/>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="3"/>
@@ -3110,7 +3110,7 @@
       <c r="E65" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F65" s="21"/>
+      <c r="F65" s="23"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="3" t="s">
@@ -3220,7 +3220,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="3"/>
-      <c r="B73" s="25" t="s">
+      <c r="B73" s="21" t="s">
         <v>95</v>
       </c>
       <c r="C73" s="16"/>
@@ -3230,10 +3230,10 @@
       <c r="E73" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F73" s="26" t="s">
+      <c r="F73" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G73" s="26" t="s">
+      <c r="G73" s="22" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>